<commit_message>
excel densidade populacional pbix jorge
</commit_message>
<xml_diff>
--- a/Arquivos/Dataset/densidade_populacional.xlsx
+++ b/Arquivos/Dataset/densidade_populacional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciellos\GymTrendTaskForce\Arquivos\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Documents\Projectos\UPskill\Projecto Power\GymTrend-Task-Force\Arquivos\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D05657-21DA-4CAB-B86B-92BB22EE356C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454DB8F0-92E5-403D-9022-BD475C0FA566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{C65B4674-CDC1-4745-B424-00CAB87FDDDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{C65B4674-CDC1-4745-B424-00CAB87FDDDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Concelho2022" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="313">
   <si>
     <t>Distrito</t>
   </si>
@@ -1402,14 +1402,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>63.7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>1500.9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>414.1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>638.6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>2901.1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>144.19999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>134.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>138.69999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>158.80000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>128.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>420.3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>245.8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>551.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>146.19999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>274.39999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>376.9</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>142.80000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>218</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>218</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>218</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>218</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>218</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>218</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>218</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>218</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>218</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>218</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>218</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>218</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>218</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>218</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>218</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>11</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>232.2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>11</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>307.60000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1071.0999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>377.5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>11</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>11</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>206.4</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>64.099999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>11</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>220.6</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>11</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>648.9</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>11</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>164.9</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>11</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>55.4</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>11</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>667.1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>11</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>978.6</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>97.2</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>64</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>64</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>64</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>64</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>64</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>142</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>142</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>142</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>142</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>142</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>142</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>33.200000000000003</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>142</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>142</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>142</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>83.2</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>142</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>100</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>100</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>100</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>444.8</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>100</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>123.2</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>100</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>156.6</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>100</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>100</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>124.1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>100</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>176.7</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>100</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>98.8</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>100</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>100</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>107.9</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>100</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>82.7</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>100</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>100</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>59.7</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>100</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>40.9</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>100</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>100</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>56.9</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>100</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>83.1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>249</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>249</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>249</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>44.3</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>249</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>249</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>41.1</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>249</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>249</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>249</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>249</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>249</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>249</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>249</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>51.2</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>249</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>249</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>263</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>319.5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>263</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>263</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>263</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>263</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>335.8</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>263</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>273.8</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>263</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>157.5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>263</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>263</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>13.6</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>263</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>340.9</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>263</v>
       </c>
@@ -2674,7 +2674,7 @@
         <v>332.7</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>263</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>263</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>263</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>263</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>263</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>309.5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>80</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>80</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>80</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>80</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>80</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>80</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>80</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>80</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>40.5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>80</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>56.1</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>80</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>80</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>80</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>80</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>80</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>80</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>119</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>119</v>
       </c>
@@ -2916,7 +2916,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>119</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>153.9</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>119</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>119</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>119</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>230.7</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>119</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>212.2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>119</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>119</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>81.900000000000006</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>119</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>89.9</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>119</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>136.9</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>119</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>146.4</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>119</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>79.7</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>119</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>204.1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>119</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>184.8</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>119</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>119</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>119</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>345.5</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>165</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>152.19999999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>165</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>187.8</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>165</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>216.7</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>165</v>
       </c>
@@ -3136,7 +3136,7 @@
         <v>209.7</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>165</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>84.2</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>165</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>7310.1</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>165</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>2196.1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>165</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>5466.5</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>165</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>1215.0999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>165</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>302.7</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>165</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>5642.2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>165</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>3755.2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>165</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>1215.4000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>165</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>433.2</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>234</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>234</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>234</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>6.3</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>234</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>234</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>12.1</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>234</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>234</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>234</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>234</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>234</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>234</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>234</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>234</v>
       </c>
@@ -3389,7 +3389,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>234</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>234</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>28</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>1260.5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>28</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>1673.5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>28</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>2813.7</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>28</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>543.20000000000005</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>28</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>5753.2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>28</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>797.6</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>28</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>495.4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>28</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>544.9</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>28</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>1297.0999999999999</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>28</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>28</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>1820.8</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>28</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>172.7</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>28</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>99.4</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>28</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>479.7</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>28</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>497.1</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>28</v>
       </c>
@@ -3587,7 +3587,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>28</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>28</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>329.3</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>177</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>47.5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>177</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>177</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>47.9</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>177</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>1536.1</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>177</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>41.3</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>177</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>177</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>108.7</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>177</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>177</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>103.8</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>177</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>127.2</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>177</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>149.19999999999999</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>177</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>177</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>74.900000000000006</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>177</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>59.7</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>177</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>150.6</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>177</v>
       </c>
@@ -3785,7 +3785,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>177</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>177</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>177</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>79.400000000000006</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>177</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>92.4</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>177</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>108.4</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>207</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>152.6</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>207</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>2544.1</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>207</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>2164.9</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>207</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>1219.5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>207</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>164.4</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>207</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>152.30000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>207</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>207</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>275.10000000000002</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>207</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>533.29999999999995</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>207</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>207</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>207</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>1</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>46.2</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>1</v>
       </c>
@@ -3994,7 +3994,7 @@
         <v>117.4</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>1</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>1</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>84.6</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>1</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>62.8</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>1</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>1</v>
       </c>
@@ -4049,7 +4049,7 @@
         <v>128.19999999999999</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>1</v>
       </c>
@@ -4060,7 +4060,7 @@
         <v>118.3</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>1</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>269.7</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>1</v>
       </c>
@@ -4082,7 +4082,7 @@
         <v>83.8</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>43</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>43</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>43</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>43</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>43</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>43</v>
       </c>
@@ -4148,7 +4148,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>43</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>43</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>48.7</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>43</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>132.30000000000001</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>43</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>43</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>152.30000000000001</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>43</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>43</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>86.8</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>43</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>54</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>54</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>54</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>146.19999999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>54</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>54</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>54</v>
       </c>
@@ -4302,7 +4302,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>54</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>54</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>54</v>
       </c>
@@ -4335,7 +4335,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>54</v>
       </c>
@@ -4346,7 +4346,7 @@
         <v>77.7</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>54</v>
       </c>
@@ -4357,7 +4357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>54</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>83.6</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>54</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>104.8</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>54</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>66.3</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>54</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>54</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>96.4</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>54</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>54</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>54</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>54</v>
       </c>
@@ -4456,7 +4456,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>54</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>197.5</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>54</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>49.9</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>279</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>56.6</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>279</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>319.89999999999998</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>279</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>43.7</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>279</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>292.2</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>279</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>55.2</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>279</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>177.1</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>279</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>279</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>141.80000000000001</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>279</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>121.8</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>279</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>67.8</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>279</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>279</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>42.2</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>279</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>279</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>43.9</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
         <v>279</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>23.4</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>279</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>83.4</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>279</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>279</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>279</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>299</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>98.3</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>299</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>620.70000000000005</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>299</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>1396.2</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
         <v>299</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>286.60000000000002</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
         <v>299</v>
       </c>
@@ -4742,7 +4742,7 @@
         <v>183.7</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" s="2" t="s">
         <v>299</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>299</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>196.2</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
         <v>299</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>531.20000000000005</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" s="2" t="s">
         <v>299</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" s="2" t="s">
         <v>299</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>61.7</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" s="2" t="s">
         <v>299</v>
       </c>
@@ -4809,7 +4809,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C279">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C279">
     <sortCondition ref="A2:A279"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4818,19 +4818,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D51B7BC-E94D-4EC5-AE0B-F4ED6A6E4633}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A21" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>254.6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>218</v>
       </c>
@@ -4854,7 +4854,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -4862,7 +4862,7 @@
         <v>315.7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>142</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>100</v>
       </c>
@@ -4886,7 +4886,7 @@
         <v>103.5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>249</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>263</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>94.5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>119</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>133.19999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>165</v>
       </c>
@@ -4926,7 +4926,7 @@
         <v>817.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>234</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>745.2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>177</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>207</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>170.3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>104.7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -4974,28 +4974,12 @@
         <v>42.8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B19" s="2">
         <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B20" s="2">
-        <v>103.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="B21" s="2">
-        <v>316.10000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>